<commit_message>
I think it's done, need commented code to be ready.
</commit_message>
<xml_diff>
--- a/report/transfer rates.xlsx
+++ b/report/transfer rates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="20940" windowHeight="10110"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="19320" windowHeight="10110"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -341,36 +341,76 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="40229888"/>
-        <c:axId val="42013440"/>
+        <c:axId val="66236416"/>
+        <c:axId val="66237952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40229888"/>
+        <c:axId val="66236416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Byte Delay</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42013440"/>
+        <c:crossAx val="66237952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42013440"/>
+        <c:axId val="66237952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Throughput (bytes/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40229888"/>
+        <c:crossAx val="66236416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -383,7 +423,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -490,47 +530,79 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="63072896"/>
-        <c:axId val="63067648"/>
+        <c:axId val="66253952"/>
+        <c:axId val="66255488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63072896"/>
+        <c:axId val="66253952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
           <c:min val="8"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Byte Delay (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63067648"/>
+        <c:crossAx val="66255488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63067648"/>
+        <c:axId val="66255488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Ratio of Good Data Transmitted to Bytes Trasmitted</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63072896"/>
+        <c:crossAx val="66253952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -541,15 +613,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>847725</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -571,14 +643,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:colOff>1076324</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -889,7 +961,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -949,7 +1021,7 @@
         <v>99</v>
       </c>
       <c r="F2">
-        <f>A2/E2</f>
+        <f t="shared" ref="F2:F8" si="0">A2/E2</f>
         <v>5.0101010101010104</v>
       </c>
       <c r="G2">
@@ -957,7 +1029,7 @@
         <v>7.5151515151515156</v>
       </c>
       <c r="H2">
-        <f>C2/E2</f>
+        <f t="shared" ref="H2:H8" si="1">C2/E2</f>
         <v>52.363636363636367</v>
       </c>
       <c r="J2">
@@ -970,7 +1042,7 @@
         <v>1040</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B8" si="0">A3*6/4</f>
+        <f t="shared" ref="B3:B8" si="2">A3*6/4</f>
         <v>1560</v>
       </c>
       <c r="C3">
@@ -983,19 +1055,19 @@
         <v>56</v>
       </c>
       <c r="F3">
-        <f>A3/E3</f>
+        <f t="shared" si="0"/>
         <v>18.571428571428573</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G7" si="1">B3/E3</f>
+        <f t="shared" ref="G3:G7" si="3">B3/E3</f>
         <v>27.857142857142858</v>
       </c>
       <c r="H3">
-        <f>C3/E3</f>
+        <f t="shared" si="1"/>
         <v>47.678571428571431</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J7" si="2">B3/C3</f>
+        <f t="shared" ref="J3:J7" si="4">B3/C3</f>
         <v>0.5842696629213483</v>
       </c>
     </row>
@@ -1004,7 +1076,7 @@
         <v>1040</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1560</v>
       </c>
       <c r="C4">
@@ -1017,19 +1089,19 @@
         <v>55</v>
       </c>
       <c r="F4">
-        <f>A4/E4</f>
+        <f t="shared" si="0"/>
         <v>18.90909090909091</v>
       </c>
       <c r="G4">
+        <f t="shared" si="3"/>
+        <v>28.363636363636363</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="1"/>
-        <v>28.363636363636363</v>
-      </c>
-      <c r="H4">
-        <f>C4/E4</f>
         <v>43.090909090909093</v>
       </c>
       <c r="J4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.65822784810126578</v>
       </c>
     </row>
@@ -1051,7 +1123,7 @@
         <v>59</v>
       </c>
       <c r="F5">
-        <f>A5/E5</f>
+        <f t="shared" si="0"/>
         <v>17.491525423728813</v>
       </c>
       <c r="G5">
@@ -1059,7 +1131,7 @@
         <v>26.237288135593221</v>
       </c>
       <c r="H5">
-        <f>C5/E5</f>
+        <f t="shared" si="1"/>
         <v>41.389830508474574</v>
       </c>
       <c r="J5">
@@ -1085,7 +1157,7 @@
         <v>59</v>
       </c>
       <c r="F6">
-        <f>A6/E6</f>
+        <f t="shared" si="0"/>
         <v>17.627118644067796</v>
       </c>
       <c r="G6">
@@ -1093,7 +1165,7 @@
         <v>26.440677966101696</v>
       </c>
       <c r="H6">
-        <f>C6/E6</f>
+        <f t="shared" si="1"/>
         <v>40.372881355932201</v>
       </c>
       <c r="J6">
@@ -1106,7 +1178,7 @@
         <v>1032</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1548</v>
       </c>
       <c r="C7">
@@ -1119,19 +1191,19 @@
         <v>60</v>
       </c>
       <c r="F7">
-        <f>A7/E7</f>
+        <f t="shared" si="0"/>
         <v>17.2</v>
       </c>
       <c r="G7">
+        <f t="shared" si="3"/>
+        <v>25.8</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="1"/>
-        <v>25.8</v>
-      </c>
-      <c r="H7">
-        <f>C7/E7</f>
         <v>38.9</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.66323907455012854</v>
       </c>
     </row>
@@ -1140,7 +1212,7 @@
         <v>1024</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1536</v>
       </c>
       <c r="C8">
@@ -1153,19 +1225,19 @@
         <v>63</v>
       </c>
       <c r="F8">
-        <f>A8/E8</f>
+        <f t="shared" si="0"/>
         <v>16.253968253968253</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8" si="3">B8/E8</f>
+        <f t="shared" ref="G8" si="5">B8/E8</f>
         <v>24.38095238095238</v>
       </c>
       <c r="H8">
-        <f>C8/E8</f>
+        <f t="shared" si="1"/>
         <v>38.476190476190474</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8" si="4">B8/C8</f>
+        <f t="shared" ref="J8" si="6">B8/C8</f>
         <v>0.63366336633663367</v>
       </c>
     </row>

</xml_diff>